<commit_message>
correction d'un bug lies au mauvais indicage dans la lecture de fichier excel
</commit_message>
<xml_diff>
--- a/Differences finies/Excel/donnee.xlsx
+++ b/Differences finies/Excel/donnee.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projet\Java\TPS-Ananum\Differences finies\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA7DF64-464C-466B-B7DE-762CA510EE74}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743205DA-7371-4FE6-BF85-4D77C45E26CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{F095363A-9AC1-4592-81AC-018AE233525F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="43">
   <si>
     <t>fonctionATester</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>erreurRel</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>0.0000000001</t>
   </si>
 </sst>
 </file>
@@ -511,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D66D300-9D4B-47E5-AF68-8C9D2A9C905C}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -521,7 +527,7 @@
     <col min="2" max="2" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -538,7 +544,7 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
@@ -552,8 +558,8 @@
       <c r="D2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E2">
-        <v>0</v>
+      <c r="E2" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>22</v>
@@ -566,8 +572,8 @@
       <c r="D3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E3">
-        <v>0</v>
+      <c r="E3" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>26</v>
@@ -580,8 +586,8 @@
       <c r="D4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E4">
-        <v>0</v>
+      <c r="E4" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>25</v>
@@ -594,8 +600,8 @@
       <c r="D5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E5">
-        <v>0</v>
+      <c r="E5" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>24</v>
@@ -608,9 +614,8 @@
       <c r="D6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E6">
-        <f>POWER(10,-10)</f>
-        <v>1E-10</v>
+      <c r="E6" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>23</v>
@@ -623,9 +628,8 @@
       <c r="D7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E7">
-        <f t="shared" ref="E7:E18" si="0">POWER(10,-10)</f>
-        <v>1E-10</v>
+      <c r="E7" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>27</v>
@@ -638,9 +642,8 @@
       <c r="D8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>1E-10</v>
+      <c r="E8" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>28</v>
@@ -653,9 +656,8 @@
       <c r="D9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>1E-10</v>
+      <c r="E9" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>29</v>
@@ -668,9 +670,8 @@
       <c r="D10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>1E-10</v>
+      <c r="E10" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>30</v>
@@ -683,9 +684,8 @@
       <c r="D11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>1E-10</v>
+      <c r="E11" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>31</v>
@@ -698,9 +698,8 @@
       <c r="D12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>1E-10</v>
+      <c r="E12" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>32</v>
@@ -713,9 +712,8 @@
       <c r="D13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>1E-10</v>
+      <c r="E13" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>37</v>
@@ -728,9 +726,8 @@
       <c r="D14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
-        <v>1E-10</v>
+      <c r="E14" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>36</v>
@@ -743,9 +740,8 @@
       <c r="D15" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>1E-10</v>
+      <c r="E15" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>33</v>
@@ -758,9 +754,8 @@
       <c r="D16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E16">
-        <f t="shared" si="0"/>
-        <v>1E-10</v>
+      <c r="E16" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>35</v>
@@ -773,9 +768,8 @@
       <c r="D17" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E17">
-        <f t="shared" si="0"/>
-        <v>1E-10</v>
+      <c r="E17" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>34</v>
@@ -788,9 +782,8 @@
       <c r="D18" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E18">
-        <f t="shared" si="0"/>
-        <v>1E-10</v>
+      <c r="E18" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>38</v>

</xml_diff>